<commit_message>
TestCase3 y correccion gramatical anteriores tc
</commit_message>
<xml_diff>
--- a/CasosDePrueba/MatrizDePrueba.xlsx
+++ b/CasosDePrueba/MatrizDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cacb292a451908e7/Desktop/ProyectoFinalQA/CasosDePrueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_F25DC773A252ABDACC10486F019D5CE45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7637E24-0CAB-4921-B567-E058966AF312}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_F25DC773A252ABDACC10486F019D5CE45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF8DEDD7-1C60-4B0B-93DE-0BBFBECD9716}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>Tester: Fernandez Victoria</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Crear publicación solo texto</t>
-  </si>
-  <si>
-    <t>Crear post solo texto</t>
   </si>
   <si>
     <t>Usuario logueado</t>
@@ -159,9 +156,6 @@
     <t>Crear publicación con imagen</t>
   </si>
   <si>
-    <t>Crear post con imagen</t>
-  </si>
-  <si>
     <t>1.Ingresar al muro o feed principal.
 2.Seleccionar el campo “¿Qué estas pensando?” 3. Adjuntar una o mas imgenes
 4.Escribir un texto (OPCIONAL)
@@ -169,6 +163,31 @@
   </si>
   <si>
     <t>El sistema debe publicar la imagen correctamente y mostrarlo en el muro del usuario</t>
+  </si>
+  <si>
+    <t>Ver publicaciones de amigos en el feed</t>
+  </si>
+  <si>
+    <t>Usuario logueado con amigos agregados</t>
+  </si>
+  <si>
+    <t>1.Ingresar a la app.
+2.Deslizar en el feed.</t>
+  </si>
+  <si>
+    <t>Dado Usuario Logueado Cuando Crea Publicación Solo Texto Entonces Publicación Exitosa</t>
+  </si>
+  <si>
+    <t>Dado Usuario Logueado Cuando Crea Publicación Con Texto e Imagen Entonces Publicación Exitosa</t>
+  </si>
+  <si>
+    <t>Dado Usuario Con Amigos Cuando Accede al Feed Entonces Visualiza Publicaciones Cronológicas</t>
+  </si>
+  <si>
+    <t>El sistema le muestra al usuario publicaciones de sus amigos ordenadas cronológicamente.</t>
+  </si>
+  <si>
+    <t>El usuario puede ver las publicaciones de sus amigos en el feed</t>
   </si>
 </sst>
 </file>
@@ -251,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -269,6 +288,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -595,7 +621,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,40 +703,40 @@
         <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="M4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="165.75" x14ac:dyDescent="0.25">
@@ -718,64 +744,88 @@
         <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="H5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="M5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="E6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -785,9 +835,9 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="F7" s="8"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="4"/>
@@ -805,9 +855,9 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="F8" s="8"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="4"/>
@@ -825,7 +875,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="6"/>
@@ -845,7 +895,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="6"/>
@@ -865,7 +915,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="6"/>
@@ -885,7 +935,7 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="6"/>
@@ -905,7 +955,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="6"/>
@@ -925,7 +975,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="6"/>
@@ -945,7 +995,7 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="6"/>
@@ -965,7 +1015,7 @@
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="6"/>
@@ -985,7 +1035,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="6"/>
@@ -1005,7 +1055,7 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="6"/>
@@ -1024,7 +1074,7 @@
       <formula>"PASA"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+  <conditionalFormatting sqref="I5:I6">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"NO PASA"</formula>
     </cfRule>

</xml_diff>